<commit_message>
updated the tables functionality
</commit_message>
<xml_diff>
--- a/website_table.xlsx
+++ b/website_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,16 +453,24 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BUY</t>
+          <t>Company</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SELL</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Change</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Value  (Rs Cr.)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -470,22 +478,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>QTY</t>
+          <t>Adani Ports</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PRICE</t>
+          <t>904.20</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PRICE</t>
+          <t>44.65</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>QTY</t>
+          <t>1,380.40</t>
         </is>
       </c>
     </row>
@@ -495,22 +503,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>ICICI Bank</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2691.00</t>
+          <t>755.85</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2695.60</t>
+          <t>3.65</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>954.20</t>
         </is>
       </c>
     </row>
@@ -520,22 +528,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>Reliance</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2690.75</t>
+          <t>2740.95</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2696.05</t>
+          <t>45.95</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>946.61</t>
         </is>
       </c>
     </row>
@@ -545,22 +553,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>HDFC Bank</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2690.70</t>
+          <t>1369.00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2696.65</t>
+          <t>3.25</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>937.55</t>
         </is>
       </c>
     </row>
@@ -570,72 +578,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>Axis Bank</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2690.65</t>
+          <t>780.40</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2696.90</t>
+          <t>-0.30</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2690.55</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2696.95</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>537.38</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added json and image download functions
</commit_message>
<xml_diff>
--- a/website_table.xlsx
+++ b/website_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,39 @@
       <c r="E1" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -453,24 +486,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Company</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Change</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Value  (Rs Cr.)</t>
-        </is>
-      </c>
+          <t>['']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -478,24 +510,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Adani Ports</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>904.20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>44.65</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1,380.40</t>
-        </is>
-      </c>
+          <t>['Index', 'Price', 'Change', '% Chg']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -503,22 +534,77 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ICICI Bank</t>
+          <t>['Nifty 50', '17082.50', '-118.30', '-0.69']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>755.85</t>
+          <t>['BSE Sensex', '56935.48', '-421.13', '-0.73']</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3.65</t>
+          <t>['Nifty Bank', '36117.10', '-287.70', '-0.79']</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>954.20</t>
+          <t>['Nifty IT', '31583.70', '-256.30', '-0.80']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['BSE SmallCap', '28808.49', '-110.34', '-0.38']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['BSE MidCap', '24558.39', '-71.86', '-0.29']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['Nifty Auto', '11130.30', '-91.50', '-0.82']</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>['BSE Cap Goods', '27300.86', '-242.01', '-0.88']</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>['BSE Cons Durable', '42951.19', '-223.09', '-0.52']</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>['BSE FMCG', '13946.77', '-41.30', '-0.30']</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>['BSE Healthcare', '24384.41', '-70.46', '-0.29']</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>['BSE Metals', '21547.92', '-104.59', '-0.48']</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>['BSE Oil Gas', '19967.69', '-84.01', '-0.42']</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>['BSE Teck', '14389.19', '-115.22', '-0.79']</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>['Nifty PSE', '4320.65', '-10.20', '-0.24']</t>
         </is>
       </c>
     </row>
@@ -528,24 +614,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Reliance</t>
+          <t>['Indices', 'Price', 'Change', '% Chg']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2740.95</t>
+          <t>['Straits Times  Apr 27', '3320.06', '-1.99', '-0.06']</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>45.95</t>
+          <t>['Hang Seng  Apr 27', '19967.84', '33.13', '0.17']</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>946.61</t>
-        </is>
-      </c>
+          <t>['Nikkei 225  Apr 27', '26345.19', '-354.92', '-1.33']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -553,24 +650,43 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>HDFC Bank</t>
+          <t>['Company', 'Price', 'Change', 'Value  (Rs Cr.)']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1369.00</t>
+          <t>['Bajaj Finance', '6981.20', '-259.35', '314.51']</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.25</t>
+          <t>['Adani Ports', '918.90', '9.40', '214.04']</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>937.55</t>
-        </is>
-      </c>
+          <t>['Reliance', '2774.85', '-0.80', '151.07']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['ICICI Bank', '747.50', '-6.25', '95.06']</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['Infosys', '1561.30', '-19.70', '92.61']</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -578,24 +694,883 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Axis Bank</t>
+          <t>['Company', 'Price', 'Change', 'Value  (Rs Cr.)']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>780.40</t>
+          <t>['Bajaj Finance', '6980.85', '-259.85', '19.51']</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>-0.30</t>
+          <t>['Reliance', '2775.05', '-0.65', '5.63']</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>537.38</t>
-        </is>
-      </c>
+          <t>['SBI', '501.60', '-4.40', '4.71']</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['HDFC Bank', '1360.55', '-11.80', '2.44']</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['Tata Steel', '1222.80', '-10.75', '1.84']</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['Company', 'Price', 'Change', '%Gain']</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['HDFC Life', '556.65', '6.80', '1.24']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['Adani Ports', '918.70', '9.20', '1.01']</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['ONGC', '167.90', '0.95', '0.57']</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['Apollo Hospital', '4,640.75', '16.70', '0.36']</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>['NTPC', '157.30', '0.30', '0.19']</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['Company', 'Price', 'Change', '%Gain']</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['Sun Pharma', '921.30', '3.05', '0.33']</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>['Reliance', '2,777.20', '1.50', '0.05']</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>['Company', 'Price', 'Change', '%Loss']</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['Bajaj Finance', '6,983.60', '-256.95', '-3.55']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['Bajaj Finserv', '15,186.00', '-248.35', '-1.61']</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['Larsen', '1,675.95', '-24.00', '-1.41']</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['UltraTechCement', '6,564.90', '-95.30', '-1.43']</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>['Grasim', '1,693.30', '-24.70', '-1.44']</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>['Company', 'Price', 'Change', '%Loss']</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['Bajaj Finance', '6,976.00', '-264.70', '-3.66']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['Bajaj Finserv', '15,178.80', '-247.55', '-1.60']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['UltraTechCement', '6,560.15', '-98.95', '-1.49']</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['Larsen', '1,675.80', '-23.70', '-1.39']</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['M M', '928.30', '-12.10', '-1.29']</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>['Commodity', 'Price', '', 'Change', '% Chg']</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['Gold Jun 03', '51,527.00', '', '-57.00', '-0.11']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['Silver May 05', '64,950.00', '', '-18.00', '-0.03']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['Crudeoil May 19', '7,832.00', '', '-37.00', '-0.47']</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['Naturalgas May 25', '537.50', '', '-7.00', '-1.29']</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>['Commodity', 'Price', '', 'Change', '% Chg']</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['Sybeanidr May 20', '0.00', '', '0.00', '']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['Cocudakl May 20', '2,863.00', '', '18.00', '0.63']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['Cocudakl May 20', '3,097.00', '', '0.00', '0.00']</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['Tmcfgrnzm May 20', '9,156.00', '', '0.00', '0.00']</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>['Currency', 'Price', 'Change', '% Chg']</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['USDINR May 27', '76.9650', '0.12', '0.15']</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['JPYINR Apr 27', '60.0625', '0.06', '0.10']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['EURINR May 27', '82.0550', '-0.27', '-0.32']</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['GBPINR Apr 27', '96.5025', '-0.98', '-1.01']</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>['Name', 'Price', 'Change', '% Chg']</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['Indiabulls Hsg', '159.90', '-2.10', '-1.3']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['Sbi', '501.25', '-4.25', '-0.84']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['Ntpc', '157.35', '0.35', '0.22']</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['Nhpc', '33.60', '-0.20', '-0.59']</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>['Equity', 'Type', 'Issue Price', 'Issue Size', 'Lot Size', 'Issue Open', 'Issue Close']</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['Campus View Profile', 'IPO', '278', '1400.14', '51', '26-04', '28-04']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['Rainbow Childre View Profile', 'IPO', '516', '1595.59', '27', '27-04', '29-04']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['Fone4 Communica View Profile', 'SME IPO', '10', '6.8', '10000', '25-04', '27-04']</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['Le Merite View Profile', 'SME IPO', '75', '48', '1600', '25-04', '28-04']</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>['Equity', 'Date of filing with Sebi']</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['Prasol Chemicals Limited DRHP \xa0 ( Prasol_Chemicals_Limited_DRHP )', '19-Apr']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['Kaynes Technology India Limited DRHP \xa0 ( Kaynes_Technology_India_Limited_DRHP )', '18-Apr']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['Senco_Gold_Limited_DRHP \xa0 ( Senco_Gold_Limited_DRHP )', '18-Apr']</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['Global Longlife Hospital And Research Limited DRHP \xa0 ( Global_Longlife_Hospital_And_Research_Limited_DRHP )', '13-Apr']</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>['Equity', 'Issue Price', 'Listing Date', 'Listing Open', 'Listing Close', 'Listing Gains %', 'CMP', 'Current Gains %']</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['Eighty Jeweller', '41', '13-04', '42.00', '44.10', '7.56', '50.00', '21.95']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['Hariom Pipe', '153', '13-04', '214.00', '224.70', '46.86', '194.05', '26.83']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['Dhyaani Tile', '51', '12-04', '57.50', '54.80', '7.45', '51.00', '0.00']</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['Veranda Learn', '137', '11-04', '171.00', '160.40', '17.08', '229.25', '67.34']</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>['Scheme', 'Fund Class', 'Info', 'Order form', 'Open Date', 'Close Date']</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['No NFO details available.']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>['Equity', 'Type', 'Issue Price', 'Issue Size', 'Lot Size', 'Subscription', 'Issue Open', 'Issue Close']</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['Shashwat Furnis View Profile', 'SME IPO', '45', '2.51', '0', '', '20-04', '25-04']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['Global Longlife View Profile', 'SME IPO', '140', '49', '0', '', '21-04', '25-04']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>['Company', 'Price', 'Stock', 'Recommendation']</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['EID Parry', '545.55', '', "Hot Stocks | Double-digit returns in Suven Pharma, EID Parry, Prakash Pipes possible in short term, here's why"]</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['JSW Energy', '344.45', '', 'Trade Spotlight | What should you do with JSW Energy, Cholamandalam Investment, Apollo Tyres, NLC India, Adani Ports today?']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['Bhansali Eng', '129.20', '', 'Bhansali Engineering: Delay in brownfield expansion caps volume growth; valuation fair']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['Action Const', '241.35', '', "Hot Stocks | Bandhan Bank, Action Construction Equipment, Ceat can give up to 15% return, here's why"]</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>['AB Capital', '116.15', '', 'Trade Spotlight | What should investors do with Aditya Birla Capital, Elgi Equipments, Adani Power, Ambuja Cements on Tuesday?']</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>['Company Name', 'Agenda']</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['Bajaj Auto', 'Audited Results Dividend']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['Kohinoor Foods', 'Rights issue']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['Hatsun Agro', 'Audited Results']</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['Syngene Intl', 'Audited Results Final Dividend']</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>['Shree Digvijay', 'Audited Results Final Dividend']</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>['Company Name', 'Agenda']</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['Schaeffler Ind', 'AGM']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['Le Lavoir', 'EGM']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['Edelweiss', 'POM']</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['Anand Projects', 'EGM']</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>['AJR Infra Tol', 'EGM']</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>['Company', 'Ratio', 'Ex-Bonus']</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['ShreeGanesh Bio', '1:1', '27-04-2022']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['Pro Fin Capital', '2:1', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['Vikram Thermo', '4:1', '12-05-2022']</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['Company', 'Old FV', 'New FV', 'Ex-Splits']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['Pro Fin Capital', '10', '1', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>['Company', 'Ratio', 'FV', 'Ex-Rights']</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['Rights details not present at the moment.']</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>['Company', '%', 'Ex-Div']</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['ABB India', '260.00', '27-04-2022']</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['Mold-Tek Pack', '120.00', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['HCL Tech', '900.00', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>['KSB Pumps', '125.00', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>['Stovec Ind', '570.00', '28-04-2022']</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>['Company Name', 'Last Price', 'Change', 'Market Cap', 'Net Sales', 'Net Profit', 'Assets']</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>['Reliance', '2774.75', '-0.90', '1,876,867.72', '245667.00', '31944.00', '595,373.00']</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['TCS', '3527.15', '-19.15', '1,290,936.90', '160341.00', '38187.00', '63,500.00']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['HDFC Bank', '1361.30', '-10.75', '755,046.31', '120858.23', '15413.68', '1,508,872.09']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['Infosys', '1561.30', '-19.70', '656,798.10', '103940.00', '21235.00', '46,063.00']</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>['ICICI Bank', '747.50', '-6.25', '519,507.71', '79118.27', '-21.72', '965,122.84']</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>['HUL', '2151.00', '2.65', '505,397.08', '45996.00', '7954.00', '43,835.00']</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
served json and images on UI
</commit_message>
<xml_diff>
--- a/website_table.xlsx
+++ b/website_table.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>